<commit_message>
Updated action items and charter
</commit_message>
<xml_diff>
--- a/Action Items/closed_action_items.xlsx
+++ b/Action Items/closed_action_items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="1940" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Item</t>
   </si>
@@ -82,6 +82,72 @@
   </si>
   <si>
     <t xml:space="preserve">Reference Steve's parts list and a bluetooth telecon tool </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BYU papers, UKFs, etc. </t>
+  </si>
+  <si>
+    <t>Lit. Rev. : Sensor Fusion/Estimation</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>Flight strategies for using visual odemetry in control loop. I believe BYU has some good papers on this.</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: Visual Odemetry</t>
+  </si>
+  <si>
+    <t>Ed</t>
+  </si>
+  <si>
+    <t>Lit. Rev: Swarm Flight</t>
+  </si>
+  <si>
+    <t>Prashant</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: SLAM</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Lit. Rev: SLAM</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Adaptive controls (L1 flight control?) evaluation needed, this is what IntelinAir uses</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: Indoor Flight/Cntrl.</t>
+  </si>
+  <si>
+    <t>Bryce</t>
+  </si>
+  <si>
+    <t>Radio beacons for localization</t>
+  </si>
+  <si>
+    <t>Lit. Rev: Radio tracking/Indoor Flight/Cntrl.</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Cheap lens parametrization, strategies for mitigating bad effects of cheap cameras</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: Visual Odometry / SLAM</t>
   </si>
 </sst>
 </file>
@@ -144,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -160,6 +226,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -627,6 +696,207 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:8" ht="60">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C6" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C7" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C10" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C11" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C12" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="45">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42262</v>
+      </c>
+      <c r="C13" s="3">
+        <v>42248</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42262</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42248</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Repo Management, action item updates
</commit_message>
<xml_diff>
--- a/Action Items/closed_action_items.xlsx
+++ b/Action Items/closed_action_items.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="5640" yWindow="1940" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Status</t>
   </si>
@@ -30,9 +31,6 @@
     <t>Owners</t>
   </si>
   <si>
-    <t>Task Level</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -72,9 +70,6 @@
     <t>Drew</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Contact Dr. Frew and James about purchasing</t>
   </si>
   <si>
@@ -87,12 +82,6 @@
     <t>Lit. Rev. : Sensor Fusion/Estimation</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
     <t>Flight strategies for using visual odemetry in control loop. I believe BYU has some good papers on this.</t>
   </si>
   <si>
@@ -156,9 +145,6 @@
     <t>Controls Team</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>Create integration team</t>
   </si>
   <si>
@@ -171,9 +157,6 @@
     <t>Nav. Team</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
     <t>Get project charter signed by appropriate parties</t>
   </si>
   <si>
@@ -184,6 +167,42 @@
   </si>
   <si>
     <t>Complete purchase orders on onboard PCs and sensors</t>
+  </si>
+  <si>
+    <t>Reflash team computer</t>
+  </si>
+  <si>
+    <t>Pixhawk Controller Modelling</t>
+  </si>
+  <si>
+    <t>Implement pixhawk controller in matlab, email script to Drew by Friday</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>Perform trade study on autopilots</t>
+  </si>
+  <si>
+    <t>Accelerometer performance, gyro performance, and computing power</t>
+  </si>
+  <si>
+    <t>Matt, Tyler, Taylor</t>
+  </si>
+  <si>
+    <t>Get quadrotor flying and pull data</t>
+  </si>
+  <si>
+    <t>Use vicon tutorial from Steve to pull data while quad is flying, import into matlab</t>
+  </si>
+  <si>
+    <t>Perception Team</t>
+  </si>
+  <si>
+    <t>Prototype and perform trade studies SLAM Algorithms on Laptop/Hardware</t>
+  </si>
+  <si>
+    <t>Presentation will be made to Dr. Frew on 9-23. RGBD and LiDAR solutions</t>
   </si>
 </sst>
 </file>
@@ -247,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -283,13 +302,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -318,11 +348,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -657,27 +690,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A15" sqref="A15:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.33203125" customWidth="1"/>
-    <col min="8" max="8" width="72.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" customWidth="1"/>
+    <col min="7" max="7" width="72.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -691,13 +723,10 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>42251</v>
@@ -706,19 +735,18 @@
         <v>42248</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>42255</v>
@@ -727,19 +755,18 @@
         <v>42248</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>42255</v>
@@ -748,17 +775,16 @@
         <v>42248</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>42256</v>
@@ -767,21 +793,18 @@
         <v>42256</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
+    </row>
+    <row r="6" spans="1:6" ht="30">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>42262</v>
@@ -790,21 +813,18 @@
         <v>42248</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>42262</v>
@@ -813,21 +833,18 @@
         <v>42248</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>42262</v>
@@ -836,21 +853,18 @@
         <v>42248</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>42262</v>
@@ -859,21 +873,18 @@
         <v>42248</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B10" s="3">
         <v>42262</v>
@@ -882,19 +893,16 @@
         <v>42248</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>42262</v>
@@ -903,19 +911,16 @@
         <v>42248</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B12" s="3">
         <v>42262</v>
@@ -924,19 +929,16 @@
         <v>42248</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B13" s="3">
         <v>42262</v>
@@ -945,21 +947,18 @@
         <v>42248</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B14" s="5">
         <v>42262</v>
@@ -968,21 +967,18 @@
         <v>42248</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5">
         <v>42263</v>
@@ -991,21 +987,18 @@
         <v>42255</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B16" s="8">
         <v>42263</v>
@@ -1014,21 +1007,18 @@
         <v>42256</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30">
-      <c r="A17" s="6" t="s">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B17" s="5">
         <v>42263</v>
@@ -1037,38 +1027,34 @@
         <v>42256</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="11">
+        <v>43</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
         <v>42268</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="5">
         <v>42263</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="D18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="5">
         <v>42263</v>
@@ -1077,36 +1063,131 @@
         <v>42256</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5">
+        <v>42263</v>
+      </c>
+      <c r="C20" s="5">
+        <v>42256</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="4" t="s">
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="10">
+        <v>42272</v>
+      </c>
+      <c r="C21" s="10">
+        <v>42270</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="B22" s="5">
+        <v>42272</v>
+      </c>
+      <c r="C22" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5">
+        <v>42270</v>
+      </c>
+      <c r="C23" s="5">
+        <v>42256</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5">
-        <v>42263</v>
-      </c>
-      <c r="B20" s="5">
-        <v>42256</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>19</v>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5">
+        <v>42276</v>
+      </c>
+      <c r="C24" s="5">
+        <v>42249</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30">
+      <c r="A25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5">
+        <v>42270</v>
+      </c>
+      <c r="C25" s="5">
+        <v>42255</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1117,4 +1198,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>